<commit_message>
Program.cs: Practically no changes RssScraper: Relaxed regular expressions (finds more links now), "exclude www.live.com" heuristic added RssSources: Added several sources (incl. Google News and Yahoo News)
git-svn-id: svn://first.ijs.si:3691/DacqPipe@166 35089d11-96e9-ae4d-82a0-4b2588c93174
</commit_message>
<xml_diff>
--- a/RssSources/reputational sources v5 mIHA.xlsx
+++ b/RssSources/reputational sources v5 mIHA.xlsx
@@ -10,14 +10,14 @@
     <sheet name="web sources" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'web sources'!$A$1:$J$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'web sources'!$A$1:$J$101</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="334">
   <si>
     <t>ABC news</t>
   </si>
@@ -850,9 +850,6 @@
     <t>http://www.boston.com/tools/rss/</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.bseindia.com/sensex/xml-data/sensexrss.xml </t>
-  </si>
-  <si>
     <t>http://www.cbc.ca/rss/</t>
   </si>
   <si>
@@ -865,9 +862,6 @@
     <t>http://english.chosun.com/rss/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">http://english.chosun.com/site/data/rss/rss.xml </t>
-  </si>
-  <si>
     <t>http://edition.cnn.com/services/rss/</t>
   </si>
   <si>
@@ -908,9 +902,6 @@
   </si>
   <si>
     <t>http://english.people.com.cn/98373/98471/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.prime-tass.com/rss/engnews_rss.xml </t>
   </si>
   <si>
     <t>RSS link (if only one)</t>
@@ -979,12 +970,79 @@
     <t>Business
 Markets</t>
   </si>
+  <si>
+    <t>http://www.reuters.com/tools/rss</t>
+  </si>
+  <si>
+    <t>http://news.sky.com/skynews/Static-Pages/RSS</t>
+  </si>
+  <si>
+    <t>http://www.economist.com/rss/</t>
+  </si>
+  <si>
+    <t>http://www.straitstimes.com/STI%2BOn%2BThe%2BGo/RSS%2BNews%2BFeed/RSS%2BNews%2BFeed.html</t>
+  </si>
+  <si>
+    <t>http://online.wsj.com/public/page/rss_news_and_feeds.html?mod=djmr_rsspodcast</t>
+  </si>
+  <si>
+    <t>http://www.ouest-france.fr
+http://www.ouest-france.fr/actu/bourse.php</t>
+  </si>
+  <si>
+    <t>http://timesofindia.indiatimes.com/rss.cms</t>
+  </si>
+  <si>
+    <t>Subscription is not free.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://content.usatoday.com/marketing/rss/index.aspx?POE=FOOTER </t>
+  </si>
+  <si>
+    <t>http://www.nytimes.com/services/xml/rss/index.html</t>
+  </si>
+  <si>
+    <t>http://thefinanser.co.uk/fsclub/rss.xml</t>
+  </si>
+  <si>
+    <t>http://www.prime-tass.com/rss/engnews_rss.xml</t>
+  </si>
+  <si>
+    <t>http://english.chosun.com/site/data/rss/rss.xml</t>
+  </si>
+  <si>
+    <t>http://www.bseindia.com/sensex/xml-data/sensexrss.xml</t>
+  </si>
+  <si>
+    <t>http://www.google.com/support/news/bin/answer.py?hl=en&amp;answer=59255</t>
+  </si>
+  <si>
+    <t>http://news.yahoo.com/rss</t>
+  </si>
+  <si>
+    <t>news.yahoo.com</t>
+  </si>
+  <si>
+    <t>Yahoo News</t>
+  </si>
+  <si>
+    <t>43b</t>
+  </si>
+  <si>
+    <t>Same as #5.</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/EconomistsView</t>
+  </si>
+  <si>
+    <t>RSS not available (the same news are served via Yahoo News RSS).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,13 +1078,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1054,7 +1123,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1082,6 +1151,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1384,13 +1486,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1523,7 @@
         <v>273</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>59</v>
@@ -1586,7 +1688,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>277</v>
+        <v>325</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>40</v>
@@ -1634,7 +1736,7 @@
         <v>77</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="3" t="s">
@@ -1661,7 +1763,7 @@
         <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="3" t="s">
@@ -1688,7 +1790,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
@@ -1738,10 +1840,10 @@
         <v>83</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>67</v>
@@ -1788,7 +1890,7 @@
         <v>88</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>67</v>
@@ -1814,7 +1916,7 @@
         <v>89</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>65</v>
@@ -1840,7 +1942,7 @@
         <v>91</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>94</v>
@@ -1866,7 +1968,7 @@
         <v>95</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>67</v>
@@ -1892,7 +1994,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>98</v>
@@ -1918,7 +2020,7 @@
         <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>40</v>
@@ -1941,7 +2043,7 @@
         <v>101</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>56</v>
@@ -1964,7 +2066,7 @@
         <v>103</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>67</v>
@@ -1990,7 +2092,7 @@
         <v>104</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>105</v>
@@ -2040,7 +2142,7 @@
         <v>108</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>67</v>
@@ -2066,7 +2168,7 @@
         <v>109</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>40</v>
@@ -2089,7 +2191,7 @@
         <v>110</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>40</v>
@@ -2133,7 +2235,7 @@
         <v>112</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>113</v>
@@ -2159,10 +2261,10 @@
         <v>114</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>40</v>
@@ -2172,29 +2274,30 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="G31" s="3" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="H31" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2209,11 +2312,14 @@
         <v>52</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E32" s="4"/>
+        <v>297</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>40</v>
@@ -2235,7 +2341,9 @@
       <c r="D33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>312</v>
+      </c>
       <c r="G33" s="3" t="s">
         <v>50</v>
       </c>
@@ -2256,7 +2364,9 @@
       <c r="D34" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>313</v>
+      </c>
       <c r="G34" s="3" t="s">
         <v>67</v>
       </c>
@@ -2280,7 +2390,9 @@
       <c r="D35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="G35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2298,7 +2410,9 @@
       <c r="D36" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>314</v>
+      </c>
       <c r="G36" s="3" t="s">
         <v>119</v>
       </c>
@@ -2322,7 +2436,9 @@
       <c r="D37" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="G37" s="3" t="s">
         <v>121</v>
       </c>
@@ -2344,11 +2460,13 @@
         <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>298</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>316</v>
+      </c>
       <c r="G38" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>40</v>
@@ -2370,7 +2488,9 @@
       <c r="D39" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>318</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>124</v>
       </c>
@@ -2392,7 +2512,10 @@
         <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>320</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>65</v>
@@ -2417,7 +2540,9 @@
       <c r="D41" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>321</v>
+      </c>
       <c r="G41" s="3" t="s">
         <v>126</v>
       </c>
@@ -2439,11 +2564,14 @@
         <v>45</v>
       </c>
       <c r="E42" s="4"/>
+      <c r="F42" s="6" t="s">
+        <v>322</v>
+      </c>
       <c r="H42" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="42.8" x14ac:dyDescent="0.25">
@@ -2459,7 +2587,9 @@
       <c r="D43" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>326</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>61</v>
       </c>
@@ -2483,7 +2613,9 @@
       <c r="D44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="3" t="s">
+        <v>333</v>
+      </c>
       <c r="G44" s="3" t="s">
         <v>62</v>
       </c>
@@ -2495,95 +2627,95 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="G45" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A45" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="F45" s="23"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="G46" s="3" t="s">
+      <c r="E47" s="12"/>
+      <c r="F47" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="G47" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H47" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I46" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="J46" s="3" t="s">
+      <c r="I47" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="G47" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E48" s="4"/>
       <c r="G48" s="3" t="s">
@@ -2593,24 +2725,24 @@
         <v>44</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E49" s="4"/>
       <c r="G49" s="3" t="s">
@@ -2620,24 +2752,24 @@
         <v>44</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E50" s="4"/>
       <c r="G50" s="3" t="s">
@@ -2647,24 +2779,24 @@
         <v>44</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E51" s="4"/>
       <c r="G51" s="3" t="s">
@@ -2674,51 +2806,53 @@
         <v>44</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
+        <v>50</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E52" s="17"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="G52" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E53" s="4"/>
       <c r="G53" s="3" t="s">
@@ -2734,126 +2868,126 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E54" s="4"/>
       <c r="G54" s="3" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E55" s="4"/>
       <c r="G55" s="3" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E56" s="4"/>
       <c r="G56" s="3" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E57" s="4"/>
       <c r="G57" s="3" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E58" s="4"/>
       <c r="G58" s="3" t="s">
@@ -2863,24 +2997,24 @@
         <v>44</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E59" s="4"/>
       <c r="G59" s="3" t="s">
@@ -2890,24 +3024,24 @@
         <v>44</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E60" s="4"/>
       <c r="G60" s="3" t="s">
@@ -2917,24 +3051,24 @@
         <v>44</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E61" s="4"/>
       <c r="G61" s="3" t="s">
@@ -2950,18 +3084,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E62" s="4"/>
       <c r="G62" s="3" t="s">
@@ -2971,24 +3105,24 @@
         <v>44</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E63" s="4"/>
       <c r="G63" s="3" t="s">
@@ -2998,24 +3132,24 @@
         <v>44</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E64" s="4"/>
       <c r="G64" s="3" t="s">
@@ -3025,7 +3159,7 @@
         <v>44</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>92</v>
@@ -3033,136 +3167,139 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E65" s="4"/>
       <c r="G65" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>47</v>
+        <v>132</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>302</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>173</v>
+        <v>63</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E66" s="4"/>
       <c r="G66" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>40</v>
+        <v>172</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E67" s="4"/>
       <c r="G67" s="3" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E68" s="4"/>
       <c r="G68" s="3" t="s">
-        <v>182</v>
+        <v>67</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="E69" s="4"/>
       <c r="G69" s="3" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>69</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>184</v>
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E70" s="4"/>
       <c r="G70" s="3" t="s">
@@ -3177,44 +3314,44 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E71" s="4"/>
       <c r="G71" s="3" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E72" s="4"/>
       <c r="G72" s="3" t="s">
-        <v>233</v>
+        <v>94</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>40</v>
@@ -3225,20 +3362,20 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E73" s="4"/>
       <c r="G73" s="3" t="s">
-        <v>82</v>
+        <v>233</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>40</v>
@@ -3249,44 +3386,47 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E74" s="4"/>
       <c r="G74" s="3" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E75" s="4"/>
+      <c r="G75" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="H75" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>70</v>
@@ -3294,68 +3434,65 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E76" s="4"/>
-      <c r="G76" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="H76" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E77" s="4"/>
+      <c r="G77" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="H77" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E78" s="4"/>
-      <c r="G78" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="H78" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>70</v>
@@ -3363,68 +3500,68 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>243</v>
+        <v>52</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E79" s="4"/>
       <c r="G79" s="3" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>52</v>
+        <v>243</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E80" s="4"/>
       <c r="G80" s="3" t="s">
-        <v>245</v>
+        <v>67</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>246</v>
+        <v>193</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E81" s="4"/>
       <c r="G81" s="3" t="s">
-        <v>67</v>
+        <v>245</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>40</v>
@@ -3435,20 +3572,20 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E82" s="4"/>
       <c r="G82" s="3" t="s">
-        <v>250</v>
+        <v>67</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>40</v>
@@ -3459,89 +3596,89 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E83" s="4"/>
+      <c r="G83" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="H83" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E84" s="4"/>
-      <c r="G84" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H84" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E85" s="6"/>
+      <c r="D85" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E85" s="4"/>
       <c r="G85" s="3" t="s">
-        <v>253</v>
+        <v>67</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E86" s="6"/>
       <c r="G86" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>56</v>
@@ -3552,20 +3689,20 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E87" s="6"/>
       <c r="G87" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>56</v>
@@ -3576,23 +3713,23 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E88" s="6"/>
       <c r="G88" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>87</v>
@@ -3600,20 +3737,20 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E89" s="6"/>
       <c r="G89" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>40</v>
@@ -3624,23 +3761,23 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>144</v>
+        <v>52</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="E90" s="6"/>
       <c r="G90" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>87</v>
@@ -3648,23 +3785,23 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>259</v>
+        <v>144</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="E91" s="6"/>
       <c r="G91" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>87</v>
@@ -3672,44 +3809,44 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>52</v>
+        <v>259</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E92" s="6"/>
       <c r="G92" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>40</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E93" s="6"/>
       <c r="G93" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>40</v>
@@ -3720,146 +3857,146 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E94" s="6"/>
       <c r="G94" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E95" s="6"/>
       <c r="G95" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E96" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E96" s="6"/>
       <c r="G96" s="3" t="s">
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I96" s="10" t="s">
-        <v>313</v>
+        <v>40</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E97" s="6"/>
+        <v>228</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E97" s="4"/>
       <c r="G97" s="3" t="s">
-        <v>266</v>
+        <v>132</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I97" s="10" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E98" s="6"/>
       <c r="G98" s="3" t="s">
         <v>266</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>310</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>226</v>
+        <v>52</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E99" s="6"/>
       <c r="G99" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>40</v>
@@ -3870,20 +4007,20 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E100" s="6"/>
       <c r="G100" s="3" t="s">
-        <v>61</v>
+        <v>267</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>40</v>
@@ -3894,30 +4031,54 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E101" s="6"/>
+      <c r="G101" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
         <v>100</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B102" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D102" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="E101" s="6"/>
-      <c r="H101" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="H102" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H100"/>
+  <autoFilter ref="A1:H101"/>
   <sortState ref="B4:E57">
     <sortCondition ref="B4"/>
   </sortState>
@@ -3935,27 +4096,27 @@
     <hyperlink ref="D38" r:id="rId11" display="http://online.wsj.com/mdc/public/page/marketsdata_europe.html"/>
     <hyperlink ref="D39" r:id="rId12"/>
     <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D45" r:id="rId14"/>
-    <hyperlink ref="D48" r:id="rId15"/>
-    <hyperlink ref="D49" r:id="rId16"/>
-    <hyperlink ref="D50" r:id="rId17"/>
-    <hyperlink ref="D51" r:id="rId18"/>
-    <hyperlink ref="D52" r:id="rId19"/>
-    <hyperlink ref="D54" r:id="rId20"/>
-    <hyperlink ref="D55" r:id="rId21"/>
-    <hyperlink ref="D57" r:id="rId22"/>
-    <hyperlink ref="D56" r:id="rId23"/>
-    <hyperlink ref="D58" r:id="rId24"/>
-    <hyperlink ref="D59" r:id="rId25"/>
-    <hyperlink ref="D60" r:id="rId26"/>
-    <hyperlink ref="D63" r:id="rId27"/>
-    <hyperlink ref="D64" r:id="rId28"/>
-    <hyperlink ref="D62" r:id="rId29"/>
-    <hyperlink ref="D65" r:id="rId30"/>
-    <hyperlink ref="D53" r:id="rId31"/>
-    <hyperlink ref="D61" r:id="rId32"/>
-    <hyperlink ref="D47" r:id="rId33"/>
-    <hyperlink ref="D46" r:id="rId34"/>
+    <hyperlink ref="D46" r:id="rId14"/>
+    <hyperlink ref="D49" r:id="rId15"/>
+    <hyperlink ref="D50" r:id="rId16"/>
+    <hyperlink ref="D51" r:id="rId17"/>
+    <hyperlink ref="D52" r:id="rId18"/>
+    <hyperlink ref="D53" r:id="rId19"/>
+    <hyperlink ref="D55" r:id="rId20"/>
+    <hyperlink ref="D56" r:id="rId21"/>
+    <hyperlink ref="D58" r:id="rId22"/>
+    <hyperlink ref="D57" r:id="rId23"/>
+    <hyperlink ref="D59" r:id="rId24"/>
+    <hyperlink ref="D60" r:id="rId25"/>
+    <hyperlink ref="D61" r:id="rId26"/>
+    <hyperlink ref="D64" r:id="rId27"/>
+    <hyperlink ref="D65" r:id="rId28"/>
+    <hyperlink ref="D63" r:id="rId29"/>
+    <hyperlink ref="D66" r:id="rId30"/>
+    <hyperlink ref="D54" r:id="rId31"/>
+    <hyperlink ref="D62" r:id="rId32"/>
+    <hyperlink ref="D48" r:id="rId33"/>
+    <hyperlink ref="D47" r:id="rId34"/>
     <hyperlink ref="D2" r:id="rId35"/>
     <hyperlink ref="D3" r:id="rId36"/>
     <hyperlink ref="D4" r:id="rId37"/>
@@ -3983,33 +4144,36 @@
     <hyperlink ref="D26" r:id="rId59"/>
     <hyperlink ref="D27" r:id="rId60"/>
     <hyperlink ref="D28" r:id="rId61"/>
-    <hyperlink ref="D66" r:id="rId62"/>
-    <hyperlink ref="D67" r:id="rId63"/>
-    <hyperlink ref="D68" r:id="rId64"/>
-    <hyperlink ref="D86" r:id="rId65" display="http://www.fitchratings.com/"/>
-    <hyperlink ref="D87" r:id="rId66" display="http://www.standardandpoors.com/"/>
-    <hyperlink ref="D88" r:id="rId67" display="http://www.banknews.com/"/>
-    <hyperlink ref="D89" r:id="rId68"/>
-    <hyperlink ref="D90" r:id="rId69"/>
-    <hyperlink ref="D91" r:id="rId70"/>
-    <hyperlink ref="D92" r:id="rId71" display="http://www.indystar.com/"/>
-    <hyperlink ref="D93" r:id="rId72"/>
-    <hyperlink ref="D94" r:id="rId73" display="http://www.bloomberg.com/"/>
-    <hyperlink ref="D85" r:id="rId74"/>
-    <hyperlink ref="D97" r:id="rId75"/>
-    <hyperlink ref="D98" r:id="rId76" display="http://www.ansa.it/web/notizie/rubriche/english/english.shtml"/>
-    <hyperlink ref="D99" r:id="rId77" display="http://www.afghannews.net/"/>
-    <hyperlink ref="D100" r:id="rId78" display="http://www.theaustralian.com.au/"/>
-    <hyperlink ref="D95" r:id="rId79"/>
-    <hyperlink ref="D96" r:id="rId80"/>
+    <hyperlink ref="D67" r:id="rId62"/>
+    <hyperlink ref="D68" r:id="rId63"/>
+    <hyperlink ref="D69" r:id="rId64"/>
+    <hyperlink ref="D87" r:id="rId65" display="http://www.fitchratings.com/"/>
+    <hyperlink ref="D88" r:id="rId66" display="http://www.standardandpoors.com/"/>
+    <hyperlink ref="D89" r:id="rId67" display="http://www.banknews.com/"/>
+    <hyperlink ref="D90" r:id="rId68"/>
+    <hyperlink ref="D91" r:id="rId69"/>
+    <hyperlink ref="D92" r:id="rId70"/>
+    <hyperlink ref="D93" r:id="rId71" display="http://www.indystar.com/"/>
+    <hyperlink ref="D94" r:id="rId72"/>
+    <hyperlink ref="D95" r:id="rId73" display="http://www.bloomberg.com/"/>
+    <hyperlink ref="D86" r:id="rId74"/>
+    <hyperlink ref="D98" r:id="rId75"/>
+    <hyperlink ref="D99" r:id="rId76" display="http://www.ansa.it/web/notizie/rubriche/english/english.shtml"/>
+    <hyperlink ref="D100" r:id="rId77" display="http://www.afghannews.net/"/>
+    <hyperlink ref="D101" r:id="rId78" display="http://www.theaustralian.com.au/"/>
+    <hyperlink ref="D96" r:id="rId79"/>
+    <hyperlink ref="D97" r:id="rId80"/>
     <hyperlink ref="F3" r:id="rId81"/>
     <hyperlink ref="F7" r:id="rId82"/>
     <hyperlink ref="F13" r:id="rId83"/>
     <hyperlink ref="E22" r:id="rId84"/>
     <hyperlink ref="F31" r:id="rId85"/>
     <hyperlink ref="D40" r:id="rId86"/>
+    <hyperlink ref="E40" r:id="rId87"/>
+    <hyperlink ref="F42" r:id="rId88"/>
+    <hyperlink ref="F47" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId87"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId90"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RssScraper: added new exclude heuristics and Atom to RSS functionality. RssSourcesBig.txt: new sources added (see also reputational sources v5 mIHA.xlsx).
git-svn-id: svn://first.ijs.si:3691/DacqPipe@257 35089d11-96e9-ae4d-82a0-4b2588c93174
</commit_message>
<xml_diff>
--- a/RssSources/reputational sources v5 mIHA.xlsx
+++ b/RssSources/reputational sources v5 mIHA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="136" windowWidth="13272" windowHeight="5638"/>
+    <workbookView xWindow="245" yWindow="190" windowWidth="13272" windowHeight="5583"/>
   </bookViews>
   <sheets>
     <sheet name="web sources" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="384">
   <si>
     <t>ABC news</t>
   </si>
@@ -460,15 +460,9 @@
     <t>Global Econ Trend Analysis</t>
   </si>
   <si>
-    <t>http://globaleconomicanalysis.blogspot.com/2010/05/shock-and-awe-part-ii-show-of-force.html</t>
-  </si>
-  <si>
     <t>Psy-Fi Blog</t>
   </si>
   <si>
-    <t>http://www.psyfitec.com/search/label/behavorial%20finance</t>
-  </si>
-  <si>
     <t>Market-Ticker</t>
   </si>
   <si>
@@ -532,9 +526,6 @@
     <t>http://www.financialarmageddon.com/</t>
   </si>
   <si>
-    <t>http://www.beuc.org/Content/Default.asp?PageID=2143</t>
-  </si>
-  <si>
     <t xml:space="preserve">Financial Services </t>
   </si>
   <si>
@@ -547,9 +538,6 @@
     <t>finance &gt;&gt; news by sector &gt;&gt; banks and finance</t>
   </si>
   <si>
-    <t>http://www.scmp.com/portal/site/SCMP/menuitem.0e28f4bc32cee73034ebbc0a53a0a0a0/?s=idx_Business</t>
-  </si>
-  <si>
     <t>Global / Asia</t>
   </si>
   <si>
@@ -640,9 +628,6 @@
     <t>Global finance</t>
   </si>
   <si>
-    <t>http://www.banknoise.com/</t>
-  </si>
-  <si>
     <t>Beppegrillo</t>
   </si>
   <si>
@@ -740,9 +725,6 @@
   </si>
   <si>
     <t>http://www.investors.com/default.aspx?fromad=1</t>
-  </si>
-  <si>
-    <t>http://www.itar-tass.com/eng/</t>
   </si>
   <si>
     <t>http://jen.jiji.com/</t>
@@ -993,9 +975,6 @@
     <t>http://timesofindia.indiatimes.com/rss.cms</t>
   </si>
   <si>
-    <t>Subscription is not free.</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://content.usatoday.com/marketing/rss/index.aspx?POE=FOOTER </t>
   </si>
   <si>
@@ -1029,20 +1008,191 @@
     <t>43b</t>
   </si>
   <si>
-    <t>Same as #5.</t>
-  </si>
-  <si>
     <t>http://feeds.feedburner.com/EconomistsView</t>
   </si>
   <si>
-    <t>RSS not available (the same news are served via Yahoo News RSS).</t>
+    <t>http://feeds.feedburner.com/wordpress/VYxj?format=xml</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/BaselineScenario?format=xml</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/JessesCafeAmericain?format=xml</t>
+  </si>
+  <si>
+    <t>http://feeds2.feedburner.com/abnormalreturns</t>
+  </si>
+  <si>
+    <t>http://feeds2.feedburner.com/MishsGlobalEconomicTrendAnalysis</t>
+  </si>
+  <si>
+    <t>http://globaleconomicanalysis.blogspot.com/</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/ThePsy-fiBlog?format=xml</t>
+  </si>
+  <si>
+    <t>http://www.psyfitec.com/</t>
+  </si>
+  <si>
+    <t>http://market-ticker.org/akcs-www?rss=Market-Ticker</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/InfectiousGreed</t>
+  </si>
+  <si>
+    <t>http://www.nakedcapitalism.com/feed/rss</t>
+  </si>
+  <si>
+    <t>http://www.econbrowser.com/index.rdf</t>
+  </si>
+  <si>
+    <t>http://gregmankiw.blogspot.com/feeds/posts/default?alt=rss</t>
+  </si>
+  <si>
+    <t>http://www.interfluidity.com/feed</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/marginalrevolution/feed</t>
+  </si>
+  <si>
+    <t>http://mjperry.blogspot.com/feeds/posts/default?alt=rss</t>
+  </si>
+  <si>
+    <t>http://www.capitalspectator.com/index.xml</t>
+  </si>
+  <si>
+    <t>http://www.devtacular.com/utilities/atomtorss/?url=http%3a%2f%2fwww.financialarmageddon.com%2fatom.xml</t>
+  </si>
+  <si>
+    <t>http://www.beuc.org/Content/Default.asp</t>
+  </si>
+  <si>
+    <t>http://www.scmp.com/portal/site/SCMP/template.JSP_INCLUDE_PAGE/page.scmp_jsp_include_page/?jsp=scmp_rss_feeds&amp;s=idx_Services&amp;ss=RSS</t>
+  </si>
+  <si>
+    <t>http://www.scmp.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.telegraph.co.uk/ </t>
+  </si>
+  <si>
+    <t>Protected against RSS Scraper</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>RSS not available</t>
+  </si>
+  <si>
+    <t>http://www.theglobeandmail.com/?service=rss</t>
+  </si>
+  <si>
+    <t>http://feeds.guardian.co.uk/theguardian/rss</t>
+  </si>
+  <si>
+    <t>http://www.haaretz.com/cmlink/haaretz-com-headlines-rss-1.263335?localLinksEnabled=false</t>
+  </si>
+  <si>
+    <t>http://www.hollywoodreporter.com/rss</t>
+  </si>
+  <si>
+    <t>http://www.hurriyetdailynews.com/rss.php</t>
+  </si>
+  <si>
+    <t>http://www.independent.co.uk/service/rss-feeds-775086.html</t>
+  </si>
+  <si>
+    <t>https://www.theice.com/rss.jhtml</t>
+  </si>
+  <si>
+    <t>http://www.itar-tass.com/en/</t>
+  </si>
+  <si>
+    <t>http://www.itar-tass.com/en/rss/all.xml</t>
+  </si>
+  <si>
+    <t>http://english.kyodonews.jp/rss/</t>
+  </si>
+  <si>
+    <t>http://www.latimes.com/about/rss/</t>
+  </si>
+  <si>
+    <t>http://news.morningstar.com/rss/rss.html</t>
+  </si>
+  <si>
+    <t>http://www.msnbc.msn.com/id/5216556/</t>
+  </si>
+  <si>
+    <t>http://www.fitchratings.com/jsp/creditdesk/ToolsAndModels.faces?context=2&amp;detail=57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSS not available </t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/WorldBankGroupPodcasts</t>
+  </si>
+  <si>
+    <t>http://www.russiabankingnews.com/rss.xml</t>
+  </si>
+  <si>
+    <t>http://www.indystar.com/rss</t>
+  </si>
+  <si>
+    <t>http://www.efinancialnews.com/about-us/rss-info</t>
+  </si>
+  <si>
+    <t>http://www.gfmag.com/rss-feeds.html</t>
+  </si>
+  <si>
+    <t>http://www.banknoise.com/en/</t>
+  </si>
+  <si>
+    <t>http://feeds.feedburner.com/banknoise?format=xml</t>
+  </si>
+  <si>
+    <t>http://www.ansa.it/web/notizie/rubriche/english/english_rss.xml</t>
+  </si>
+  <si>
+    <t>http://www.theaustralian.com.au/help/rss</t>
+  </si>
+  <si>
+    <t>http://www.fin24.com/About/Rss-Feeds</t>
+  </si>
+  <si>
+    <t>Seeking Alpha</t>
+  </si>
+  <si>
+    <t>http://seekingalpha.com/</t>
+  </si>
+  <si>
+    <t>http://seekingalpha.com/page/feeds</t>
+  </si>
+  <si>
+    <t>Same as #5</t>
+  </si>
+  <si>
+    <t>RSS not available (the same news are served via Yahoo News RSS)</t>
+  </si>
+  <si>
+    <t>Subscription is not free</t>
+  </si>
+  <si>
+    <t>This Web site seems to be dead</t>
+  </si>
+  <si>
+    <t>http://www.devtacular.com/utilities/atomtorss/?url=http%3a%2f%2ffeeds.feedburner.com%2fCalculatedRisk</t>
+  </si>
+  <si>
+    <t>http://www.devtacular.com/utilities/atomtorss/?url=http%3a%2f%2ffeeds.feedburner.com%2fbrontecapital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1083,8 +1233,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1094,6 +1257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1123,7 +1292,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1184,6 +1353,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1486,13 +1670,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomRight" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1520,10 +1704,10 @@
         <v>28</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>59</v>
@@ -1552,7 +1736,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="3" t="s">
@@ -1580,7 +1764,7 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>67</v>
@@ -1606,7 +1790,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
@@ -1633,7 +1817,7 @@
         <v>71</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="3" t="s">
@@ -1660,7 +1844,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="3" t="s">
@@ -1688,7 +1872,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>40</v>
@@ -1736,7 +1920,7 @@
         <v>77</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="3" t="s">
@@ -1763,7 +1947,7 @@
         <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="3" t="s">
@@ -1790,7 +1974,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
@@ -1840,10 +2024,10 @@
         <v>83</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>67</v>
@@ -1890,7 +2074,7 @@
         <v>88</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>67</v>
@@ -1916,7 +2100,7 @@
         <v>89</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>65</v>
@@ -1942,7 +2126,7 @@
         <v>91</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>94</v>
@@ -1968,7 +2152,7 @@
         <v>95</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>67</v>
@@ -1994,7 +2178,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>98</v>
@@ -2020,7 +2204,7 @@
         <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>40</v>
@@ -2043,7 +2227,7 @@
         <v>101</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>56</v>
@@ -2066,7 +2250,7 @@
         <v>103</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>67</v>
@@ -2092,7 +2276,7 @@
         <v>104</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>105</v>
@@ -2142,7 +2326,7 @@
         <v>108</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>67</v>
@@ -2168,7 +2352,7 @@
         <v>109</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>40</v>
@@ -2191,7 +2375,7 @@
         <v>110</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>40</v>
@@ -2235,7 +2419,7 @@
         <v>112</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>113</v>
@@ -2261,10 +2445,10 @@
         <v>114</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>40</v>
@@ -2288,7 +2472,7 @@
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="13" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>116</v>
@@ -2312,14 +2496,14 @@
         <v>52</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>40</v>
@@ -2342,7 +2526,7 @@
         <v>51</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>50</v>
@@ -2365,7 +2549,7 @@
         <v>117</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>67</v>
@@ -2391,7 +2575,7 @@
         <v>46</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>42</v>
@@ -2411,7 +2595,7 @@
         <v>118</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>119</v>
@@ -2436,8 +2620,8 @@
       <c r="D37" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>319</v>
+      <c r="E37" s="25" t="s">
+        <v>380</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>121</v>
@@ -2460,13 +2644,13 @@
         <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>40</v>
@@ -2489,7 +2673,7 @@
         <v>123</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>124</v>
@@ -2512,10 +2696,10 @@
         <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>65</v>
@@ -2541,7 +2725,7 @@
         <v>125</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>126</v>
@@ -2565,13 +2749,13 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="42.8" x14ac:dyDescent="0.25">
@@ -2588,7 +2772,7 @@
         <v>60</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>61</v>
@@ -2613,8 +2797,8 @@
       <c r="D44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>333</v>
+      <c r="E44" s="32" t="s">
+        <v>379</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>62</v>
@@ -2628,19 +2812,19 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="21"/>
@@ -2661,8 +2845,8 @@
       <c r="D46" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>331</v>
+      <c r="E46" s="25" t="s">
+        <v>378</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>129</v>
@@ -2689,7 +2873,7 @@
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="13" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>132</v>
@@ -2698,7 +2882,7 @@
         <v>44</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J47" s="11" t="s">
         <v>87</v>
@@ -2718,6 +2902,9 @@
         <v>134</v>
       </c>
       <c r="E48" s="4"/>
+      <c r="F48" s="6" t="s">
+        <v>325</v>
+      </c>
       <c r="G48" s="3" t="s">
         <v>132</v>
       </c>
@@ -2725,7 +2912,7 @@
         <v>44</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>70</v>
@@ -2745,6 +2932,9 @@
         <v>136</v>
       </c>
       <c r="E49" s="4"/>
+      <c r="F49" s="6" t="s">
+        <v>382</v>
+      </c>
       <c r="G49" s="3" t="s">
         <v>132</v>
       </c>
@@ -2752,7 +2942,7 @@
         <v>44</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>70</v>
@@ -2772,6 +2962,9 @@
         <v>138</v>
       </c>
       <c r="E50" s="4"/>
+      <c r="F50" s="6" t="s">
+        <v>326</v>
+      </c>
       <c r="G50" s="3" t="s">
         <v>132</v>
       </c>
@@ -2779,7 +2972,7 @@
         <v>44</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>70</v>
@@ -2799,6 +2992,9 @@
         <v>140</v>
       </c>
       <c r="E51" s="4"/>
+      <c r="F51" s="6" t="s">
+        <v>327</v>
+      </c>
       <c r="G51" s="3" t="s">
         <v>132</v>
       </c>
@@ -2806,7 +3002,7 @@
         <v>44</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>70</v>
@@ -2826,7 +3022,9 @@
         <v>142</v>
       </c>
       <c r="E52" s="17"/>
-      <c r="F52" s="18"/>
+      <c r="F52" s="24" t="s">
+        <v>383</v>
+      </c>
       <c r="G52" s="16" t="s">
         <v>132</v>
       </c>
@@ -2834,7 +3032,7 @@
         <v>44</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>70</v>
@@ -2855,6 +3053,9 @@
         <v>145</v>
       </c>
       <c r="E53" s="4"/>
+      <c r="F53" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="G53" s="3" t="s">
         <v>132</v>
       </c>
@@ -2862,13 +3063,13 @@
         <v>44</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2879,9 +3080,12 @@
         <v>144</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>147</v>
+        <v>330</v>
       </c>
       <c r="E54" s="4"/>
+      <c r="F54" s="6" t="s">
+        <v>329</v>
+      </c>
       <c r="G54" s="3" t="s">
         <v>132</v>
       </c>
@@ -2889,7 +3093,7 @@
         <v>44</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>70</v>
@@ -2900,15 +3104,18 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>149</v>
+        <v>332</v>
       </c>
       <c r="E55" s="4"/>
+      <c r="F55" s="6" t="s">
+        <v>331</v>
+      </c>
       <c r="G55" s="3" t="s">
         <v>62</v>
       </c>
@@ -2916,7 +3123,7 @@
         <v>44</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>70</v>
@@ -2927,15 +3134,18 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E56" s="4"/>
+      <c r="F56" s="6" t="s">
+        <v>333</v>
+      </c>
       <c r="G56" s="3" t="s">
         <v>132</v>
       </c>
@@ -2943,7 +3153,7 @@
         <v>44</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>70</v>
@@ -2954,23 +3164,26 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E57" s="4"/>
+      <c r="F57" s="6" t="s">
+        <v>335</v>
+      </c>
       <c r="G57" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>70</v>
@@ -2981,15 +3194,18 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E58" s="4"/>
+      <c r="F58" s="6" t="s">
+        <v>334</v>
+      </c>
       <c r="G58" s="3" t="s">
         <v>132</v>
       </c>
@@ -2997,7 +3213,7 @@
         <v>44</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>92</v>
@@ -3008,15 +3224,18 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E59" s="4"/>
+      <c r="F59" s="6" t="s">
+        <v>336</v>
+      </c>
       <c r="G59" s="3" t="s">
         <v>132</v>
       </c>
@@ -3024,7 +3243,7 @@
         <v>44</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>92</v>
@@ -3035,15 +3254,18 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E60" s="4"/>
+      <c r="F60" s="6" t="s">
+        <v>337</v>
+      </c>
       <c r="G60" s="3" t="s">
         <v>132</v>
       </c>
@@ -3051,7 +3273,7 @@
         <v>44</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>92</v>
@@ -3062,15 +3284,18 @@
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E61" s="4"/>
+      <c r="F61" s="6" t="s">
+        <v>338</v>
+      </c>
       <c r="G61" s="3" t="s">
         <v>132</v>
       </c>
@@ -3078,7 +3303,7 @@
         <v>44</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>92</v>
@@ -3089,15 +3314,18 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E62" s="4"/>
+      <c r="F62" s="6" t="s">
+        <v>339</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>132</v>
       </c>
@@ -3105,7 +3333,7 @@
         <v>44</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>92</v>
@@ -3116,15 +3344,18 @@
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E63" s="4"/>
+      <c r="F63" s="6" t="s">
+        <v>340</v>
+      </c>
       <c r="G63" s="3" t="s">
         <v>132</v>
       </c>
@@ -3132,7 +3363,7 @@
         <v>44</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>92</v>
@@ -3143,15 +3374,18 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E64" s="4"/>
+      <c r="F64" s="6" t="s">
+        <v>341</v>
+      </c>
       <c r="G64" s="3" t="s">
         <v>132</v>
       </c>
@@ -3159,26 +3393,29 @@
         <v>44</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E65" s="4"/>
+      <c r="F65" s="4" t="s">
+        <v>342</v>
+      </c>
       <c r="G65" s="3" t="s">
         <v>132</v>
       </c>
@@ -3186,7 +3423,7 @@
         <v>44</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>92</v>
@@ -3203,11 +3440,14 @@
         <v>52</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E66" s="4"/>
+        <v>343</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="F66" s="14"/>
       <c r="G66" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>47</v>
@@ -3221,17 +3461,20 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E67" s="4"/>
+        <v>171</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F67" s="6"/>
       <c r="G67" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>40</v>
@@ -3245,15 +3488,20 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E68" s="4"/>
+        <v>345</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>347</v>
+      </c>
       <c r="G68" s="3" t="s">
         <v>67</v>
       </c>
@@ -3269,17 +3517,19 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E69" s="4"/>
+        <v>177</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>348</v>
+      </c>
       <c r="G69" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>40</v>
@@ -3293,15 +3543,18 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E70" s="4"/>
+      <c r="F70" s="6" t="s">
+        <v>350</v>
+      </c>
       <c r="G70" s="3" t="s">
         <v>67</v>
       </c>
@@ -3317,15 +3570,18 @@
         <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E71" s="4"/>
+      <c r="F71" s="6" t="s">
+        <v>351</v>
+      </c>
       <c r="G71" s="3" t="s">
         <v>67</v>
       </c>
@@ -3341,15 +3597,18 @@
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E72" s="4"/>
+      <c r="F72" s="6" t="s">
+        <v>352</v>
+      </c>
       <c r="G72" s="3" t="s">
         <v>94</v>
       </c>
@@ -3365,17 +3624,19 @@
         <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E73" s="4"/>
+        <v>227</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>353</v>
+      </c>
       <c r="G73" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>40</v>
@@ -3389,15 +3650,18 @@
         <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E74" s="4"/>
+      <c r="F74" s="6" t="s">
+        <v>354</v>
+      </c>
       <c r="G74" s="3" t="s">
         <v>82</v>
       </c>
@@ -3413,15 +3677,17 @@
         <v>73</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E75" s="4"/>
+        <v>231</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="G75" s="3" t="s">
         <v>67</v>
       </c>
@@ -3437,15 +3703,17 @@
         <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E76" s="4"/>
+        <v>232</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>356</v>
+      </c>
       <c r="H76" s="3" t="s">
         <v>56</v>
       </c>
@@ -3458,17 +3726,19 @@
         <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="E77" s="4"/>
+        <v>233</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>349</v>
+      </c>
       <c r="G77" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>40</v>
@@ -3482,15 +3752,18 @@
         <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E78" s="4"/>
+      <c r="F78" s="26" t="s">
+        <v>347</v>
+      </c>
       <c r="H78" s="3" t="s">
         <v>56</v>
       </c>
@@ -3503,15 +3776,18 @@
         <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>241</v>
+        <v>357</v>
       </c>
       <c r="E79" s="4"/>
+      <c r="F79" s="6" t="s">
+        <v>358</v>
+      </c>
       <c r="G79" s="3" t="s">
         <v>105</v>
       </c>
@@ -3527,15 +3803,17 @@
         <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E80" s="4"/>
+        <v>236</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>349</v>
+      </c>
       <c r="G80" s="3" t="s">
         <v>67</v>
       </c>
@@ -3546,22 +3824,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E81" s="4"/>
+        <v>238</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="G81" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>40</v>
@@ -3570,20 +3850,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="E82" s="4"/>
+        <v>241</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>360</v>
+      </c>
       <c r="G82" s="3" t="s">
         <v>67</v>
       </c>
@@ -3594,139 +3876,169 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="16">
         <v>81</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="F83" s="18"/>
+      <c r="G83" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="16">
+        <v>82</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="F84" s="18"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="16">
+        <v>83</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="G85" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H85" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="16">
+        <v>84</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="F86" s="18"/>
+      <c r="G86" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="H86" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="16">
+        <v>85</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C87" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E87" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="F87" s="18"/>
+      <c r="G87" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E83" s="4"/>
-      <c r="G83" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
-        <v>82</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="H84" s="3" t="s">
+      <c r="H87" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J84" s="3" t="s">
+      <c r="I87" s="16"/>
+      <c r="J87" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
-        <v>83</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E85" s="4"/>
-      <c r="G85" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
-        <v>84</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E86" s="6"/>
-      <c r="G86" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
-        <v>85</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E87" s="6"/>
-      <c r="G87" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="16"/>
+      <c r="L87" s="16"/>
+      <c r="M87" s="16"/>
+      <c r="N87" s="16"/>
+      <c r="O87" s="16"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>86</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E88" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>364</v>
+      </c>
       <c r="G88" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>56</v>
@@ -3735,22 +4047,24 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E89" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>364</v>
+      </c>
       <c r="G89" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>40</v>
@@ -3759,22 +4073,25 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>88</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E90" s="6"/>
+      <c r="F90" s="6" t="s">
+        <v>365</v>
+      </c>
       <c r="G90" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>40</v>
@@ -3783,22 +4100,24 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>89</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="E91" s="6"/>
+        <v>251</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>364</v>
+      </c>
       <c r="G91" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>56</v>
@@ -3807,22 +4126,25 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>90</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E92" s="6"/>
+      <c r="F92" s="6" t="s">
+        <v>366</v>
+      </c>
       <c r="G92" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>40</v>
@@ -3831,22 +4153,24 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>91</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E93" s="6"/>
+        <v>197</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>367</v>
+      </c>
       <c r="G93" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>40</v>
@@ -3855,22 +4179,24 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>92</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E94" s="6"/>
+        <v>198</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>368</v>
+      </c>
       <c r="G94" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>40</v>
@@ -3879,22 +4205,24 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>93</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E95" s="6"/>
+        <v>199</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>364</v>
+      </c>
       <c r="G95" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>56</v>
@@ -3903,22 +4231,24 @@
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>94</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E96" s="6"/>
+        <v>201</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>369</v>
+      </c>
       <c r="G96" s="3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>40</v>
@@ -3932,15 +4262,17 @@
         <v>95</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E97" s="4"/>
+        <v>259</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>381</v>
+      </c>
       <c r="G97" s="3" t="s">
         <v>132</v>
       </c>
@@ -3948,7 +4280,7 @@
         <v>44</v>
       </c>
       <c r="I97" s="10" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>92</v>
@@ -3959,23 +4291,26 @@
         <v>96</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>207</v>
+        <v>370</v>
       </c>
       <c r="E98" s="6"/>
+      <c r="F98" s="6" t="s">
+        <v>371</v>
+      </c>
       <c r="G98" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I98" s="10" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>87</v>
@@ -3986,17 +4321,20 @@
         <v>97</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E99" s="6"/>
+      <c r="F99" s="6" t="s">
+        <v>372</v>
+      </c>
       <c r="G99" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>40</v>
@@ -4010,17 +4348,19 @@
         <v>98</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="D100" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E100" s="6"/>
+        <v>205</v>
+      </c>
+      <c r="E100" s="28" t="s">
+        <v>381</v>
+      </c>
       <c r="G100" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>40</v>
@@ -4034,15 +4374,17 @@
         <v>99</v>
       </c>
       <c r="B101" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="D101" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E101" s="6"/>
+        <v>206</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>373</v>
+      </c>
       <c r="G101" s="3" t="s">
         <v>61</v>
       </c>
@@ -4058,15 +4400,17 @@
         <v>100</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="E102" s="6"/>
+        <v>263</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>374</v>
+      </c>
       <c r="H102" s="3" t="s">
         <v>40</v>
       </c>
@@ -4075,7 +4419,24 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B103" s="6"/>
+      <c r="A103" s="21">
+        <v>101</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>375</v>
+      </c>
+      <c r="C103" s="21"/>
+      <c r="D103" s="31" t="s">
+        <v>376</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="F103" s="23"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+      <c r="J103" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H101"/>
@@ -4102,78 +4463,103 @@
     <hyperlink ref="D51" r:id="rId17"/>
     <hyperlink ref="D52" r:id="rId18"/>
     <hyperlink ref="D53" r:id="rId19"/>
-    <hyperlink ref="D55" r:id="rId20"/>
-    <hyperlink ref="D56" r:id="rId21"/>
-    <hyperlink ref="D58" r:id="rId22"/>
-    <hyperlink ref="D57" r:id="rId23"/>
-    <hyperlink ref="D59" r:id="rId24"/>
-    <hyperlink ref="D60" r:id="rId25"/>
-    <hyperlink ref="D61" r:id="rId26"/>
-    <hyperlink ref="D64" r:id="rId27"/>
-    <hyperlink ref="D65" r:id="rId28"/>
-    <hyperlink ref="D63" r:id="rId29"/>
-    <hyperlink ref="D66" r:id="rId30"/>
-    <hyperlink ref="D54" r:id="rId31"/>
-    <hyperlink ref="D62" r:id="rId32"/>
-    <hyperlink ref="D48" r:id="rId33"/>
-    <hyperlink ref="D47" r:id="rId34"/>
-    <hyperlink ref="D2" r:id="rId35"/>
-    <hyperlink ref="D3" r:id="rId36"/>
-    <hyperlink ref="D4" r:id="rId37"/>
-    <hyperlink ref="D5" r:id="rId38"/>
-    <hyperlink ref="D6" r:id="rId39"/>
-    <hyperlink ref="D7" r:id="rId40"/>
-    <hyperlink ref="D8" r:id="rId41"/>
-    <hyperlink ref="D9" r:id="rId42"/>
-    <hyperlink ref="D10" r:id="rId43"/>
-    <hyperlink ref="D11" r:id="rId44"/>
-    <hyperlink ref="D12" r:id="rId45"/>
-    <hyperlink ref="D13" r:id="rId46"/>
-    <hyperlink ref="D14" r:id="rId47"/>
-    <hyperlink ref="D15" r:id="rId48"/>
-    <hyperlink ref="D16" r:id="rId49"/>
-    <hyperlink ref="D17" r:id="rId50"/>
-    <hyperlink ref="D18" r:id="rId51"/>
-    <hyperlink ref="D19" r:id="rId52"/>
-    <hyperlink ref="D20" r:id="rId53"/>
-    <hyperlink ref="D21" r:id="rId54"/>
-    <hyperlink ref="D22" r:id="rId55"/>
-    <hyperlink ref="D23" r:id="rId56"/>
-    <hyperlink ref="D24" r:id="rId57"/>
-    <hyperlink ref="D25" r:id="rId58"/>
-    <hyperlink ref="D26" r:id="rId59"/>
-    <hyperlink ref="D27" r:id="rId60"/>
-    <hyperlink ref="D28" r:id="rId61"/>
-    <hyperlink ref="D67" r:id="rId62"/>
-    <hyperlink ref="D68" r:id="rId63"/>
-    <hyperlink ref="D69" r:id="rId64"/>
-    <hyperlink ref="D87" r:id="rId65" display="http://www.fitchratings.com/"/>
-    <hyperlink ref="D88" r:id="rId66" display="http://www.standardandpoors.com/"/>
-    <hyperlink ref="D89" r:id="rId67" display="http://www.banknews.com/"/>
-    <hyperlink ref="D90" r:id="rId68"/>
-    <hyperlink ref="D91" r:id="rId69"/>
-    <hyperlink ref="D92" r:id="rId70"/>
-    <hyperlink ref="D93" r:id="rId71" display="http://www.indystar.com/"/>
-    <hyperlink ref="D94" r:id="rId72"/>
-    <hyperlink ref="D95" r:id="rId73" display="http://www.bloomberg.com/"/>
-    <hyperlink ref="D86" r:id="rId74"/>
-    <hyperlink ref="D98" r:id="rId75"/>
-    <hyperlink ref="D99" r:id="rId76" display="http://www.ansa.it/web/notizie/rubriche/english/english.shtml"/>
-    <hyperlink ref="D100" r:id="rId77" display="http://www.afghannews.net/"/>
-    <hyperlink ref="D101" r:id="rId78" display="http://www.theaustralian.com.au/"/>
-    <hyperlink ref="D96" r:id="rId79"/>
-    <hyperlink ref="D97" r:id="rId80"/>
-    <hyperlink ref="F3" r:id="rId81"/>
-    <hyperlink ref="F7" r:id="rId82"/>
-    <hyperlink ref="F13" r:id="rId83"/>
-    <hyperlink ref="E22" r:id="rId84"/>
-    <hyperlink ref="F31" r:id="rId85"/>
-    <hyperlink ref="D40" r:id="rId86"/>
-    <hyperlink ref="E40" r:id="rId87"/>
-    <hyperlink ref="F42" r:id="rId88"/>
-    <hyperlink ref="F47" r:id="rId89"/>
+    <hyperlink ref="D56" r:id="rId20"/>
+    <hyperlink ref="D58" r:id="rId21"/>
+    <hyperlink ref="D57" r:id="rId22"/>
+    <hyperlink ref="D60" r:id="rId23"/>
+    <hyperlink ref="D61" r:id="rId24"/>
+    <hyperlink ref="D64" r:id="rId25"/>
+    <hyperlink ref="D65" r:id="rId26"/>
+    <hyperlink ref="D63" r:id="rId27"/>
+    <hyperlink ref="D66" r:id="rId28"/>
+    <hyperlink ref="D54" r:id="rId29"/>
+    <hyperlink ref="D62" r:id="rId30"/>
+    <hyperlink ref="D48" r:id="rId31"/>
+    <hyperlink ref="D47" r:id="rId32"/>
+    <hyperlink ref="D2" r:id="rId33"/>
+    <hyperlink ref="D3" r:id="rId34"/>
+    <hyperlink ref="D4" r:id="rId35"/>
+    <hyperlink ref="D5" r:id="rId36"/>
+    <hyperlink ref="D6" r:id="rId37"/>
+    <hyperlink ref="D7" r:id="rId38"/>
+    <hyperlink ref="D8" r:id="rId39"/>
+    <hyperlink ref="D9" r:id="rId40"/>
+    <hyperlink ref="D10" r:id="rId41"/>
+    <hyperlink ref="D11" r:id="rId42"/>
+    <hyperlink ref="D12" r:id="rId43"/>
+    <hyperlink ref="D13" r:id="rId44"/>
+    <hyperlink ref="D14" r:id="rId45"/>
+    <hyperlink ref="D15" r:id="rId46"/>
+    <hyperlink ref="D16" r:id="rId47"/>
+    <hyperlink ref="D17" r:id="rId48"/>
+    <hyperlink ref="D18" r:id="rId49"/>
+    <hyperlink ref="D19" r:id="rId50"/>
+    <hyperlink ref="D20" r:id="rId51"/>
+    <hyperlink ref="D21" r:id="rId52"/>
+    <hyperlink ref="D22" r:id="rId53"/>
+    <hyperlink ref="D23" r:id="rId54"/>
+    <hyperlink ref="D24" r:id="rId55"/>
+    <hyperlink ref="D25" r:id="rId56"/>
+    <hyperlink ref="D26" r:id="rId57"/>
+    <hyperlink ref="D27" r:id="rId58"/>
+    <hyperlink ref="D28" r:id="rId59"/>
+    <hyperlink ref="D67" r:id="rId60"/>
+    <hyperlink ref="D68" r:id="rId61"/>
+    <hyperlink ref="D69" r:id="rId62"/>
+    <hyperlink ref="D87" r:id="rId63" display="http://www.fitchratings.com/"/>
+    <hyperlink ref="D88" r:id="rId64" display="http://www.standardandpoors.com/"/>
+    <hyperlink ref="D89" r:id="rId65" display="http://www.banknews.com/"/>
+    <hyperlink ref="D90" r:id="rId66"/>
+    <hyperlink ref="D91" r:id="rId67"/>
+    <hyperlink ref="D92" r:id="rId68"/>
+    <hyperlink ref="D93" r:id="rId69" display="http://www.indystar.com/"/>
+    <hyperlink ref="D94" r:id="rId70"/>
+    <hyperlink ref="D95" r:id="rId71" display="http://www.bloomberg.com/"/>
+    <hyperlink ref="D86" r:id="rId72"/>
+    <hyperlink ref="D99" r:id="rId73" display="http://www.ansa.it/web/notizie/rubriche/english/english.shtml"/>
+    <hyperlink ref="D100" r:id="rId74" display="http://www.afghannews.net/"/>
+    <hyperlink ref="D101" r:id="rId75" display="http://www.theaustralian.com.au/"/>
+    <hyperlink ref="D96" r:id="rId76"/>
+    <hyperlink ref="D97" r:id="rId77"/>
+    <hyperlink ref="F3" r:id="rId78"/>
+    <hyperlink ref="F7" r:id="rId79"/>
+    <hyperlink ref="F13" r:id="rId80"/>
+    <hyperlink ref="E22" r:id="rId81"/>
+    <hyperlink ref="F31" r:id="rId82"/>
+    <hyperlink ref="D40" r:id="rId83"/>
+    <hyperlink ref="E40" r:id="rId84"/>
+    <hyperlink ref="F42" r:id="rId85"/>
+    <hyperlink ref="F47" r:id="rId86"/>
+    <hyperlink ref="F48" r:id="rId87"/>
+    <hyperlink ref="F50" r:id="rId88"/>
+    <hyperlink ref="F51" r:id="rId89"/>
+    <hyperlink ref="F53" r:id="rId90"/>
+    <hyperlink ref="F54" r:id="rId91"/>
+    <hyperlink ref="F55" r:id="rId92"/>
+    <hyperlink ref="F56" r:id="rId93"/>
+    <hyperlink ref="F57" r:id="rId94"/>
+    <hyperlink ref="F58" r:id="rId95"/>
+    <hyperlink ref="D59" r:id="rId96"/>
+    <hyperlink ref="F59" r:id="rId97"/>
+    <hyperlink ref="F60" r:id="rId98"/>
+    <hyperlink ref="F61" r:id="rId99"/>
+    <hyperlink ref="F62" r:id="rId100"/>
+    <hyperlink ref="F63" r:id="rId101"/>
+    <hyperlink ref="F64" r:id="rId102"/>
+    <hyperlink ref="F65" r:id="rId103"/>
+    <hyperlink ref="F70" r:id="rId104"/>
+    <hyperlink ref="F71" r:id="rId105"/>
+    <hyperlink ref="F72" r:id="rId106"/>
+    <hyperlink ref="E73" r:id="rId107"/>
+    <hyperlink ref="F74" r:id="rId108"/>
+    <hyperlink ref="D79" r:id="rId109"/>
+    <hyperlink ref="F79" r:id="rId110"/>
+    <hyperlink ref="F90" r:id="rId111"/>
+    <hyperlink ref="F92" r:id="rId112"/>
+    <hyperlink ref="F98" r:id="rId113"/>
+    <hyperlink ref="F99" r:id="rId114"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId90"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId115"/>
 </worksheet>
 </file>
</xml_diff>